<commit_message>
pushed new requirements (sorry its on dashboard)
</commit_message>
<xml_diff>
--- a/documentation/2-planning/Project Schedule.xlsx
+++ b/documentation/2-planning/Project Schedule.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51D7919-547E-004A-BC56-D03193DBECDD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F25D5D5-4616-9541-A92B-45DAD659E378}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="460" windowWidth="27720" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,22 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
-  <si>
-    <t>Task 3</t>
-  </si>
-  <si>
-    <t>Task 4</t>
-  </si>
-  <si>
-    <t>Task 5</t>
-  </si>
-  <si>
-    <t>Task 1</t>
-  </si>
-  <si>
-    <t>Task 2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -258,9 +243,6 @@
     <t>Step 4</t>
   </si>
   <si>
-    <t>Login Feature</t>
-  </si>
-  <si>
     <t>Begin Database Front-end Functionality</t>
   </si>
   <si>
@@ -270,7 +252,49 @@
     <t>Use Case, Activity Diagram, Class Diagram - Database functionality</t>
   </si>
   <si>
-    <t>Admin control interface</t>
+    <t>Test Plan</t>
+  </si>
+  <si>
+    <t>Login/Logout Feature</t>
+  </si>
+  <si>
+    <t>Database Front-End Functionality</t>
+  </si>
+  <si>
+    <t>Daniel Watson</t>
+  </si>
+  <si>
+    <t>Program Statistics Dashboard</t>
+  </si>
+  <si>
+    <t>Class Diagram</t>
+  </si>
+  <si>
+    <t>Implement tests</t>
+  </si>
+  <si>
+    <t>Jaisal Friedman, Daniel Watson</t>
+  </si>
+  <si>
+    <t>Bug Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalize Documentation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make Presentation </t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>Admin interface</t>
+  </si>
+  <si>
+    <t>Jaisal Friedman, Daniel Watson, Gabriel Garcia</t>
+  </si>
+  <si>
+    <t>Mai Oudah</t>
   </si>
 </sst>
 </file>
@@ -681,7 +705,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -884,9 +908,6 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="11" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="11" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -895,9 +916,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="11">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="12" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -905,9 +923,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="12">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="7" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="11" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -917,6 +932,19 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="11" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -929,18 +957,20 @@
     <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="12" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="12" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1541,8 +1571,8 @@
   <dimension ref="A1:AJ36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1561,10 +1591,10 @@
   <sheetData>
     <row r="1" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="59" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B1" s="63" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1572,347 +1602,350 @@
       <c r="F1" s="47"/>
       <c r="H1" s="2"/>
       <c r="I1" s="14"/>
+      <c r="K1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="2" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B2" s="64" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="58" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="79" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="87" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="88"/>
-      <c r="E3" s="83">
-        <f ca="1">TODAY()-4</f>
-        <v>43792</v>
-      </c>
-      <c r="F3" s="83"/>
+        <v>30</v>
+      </c>
+      <c r="B3" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="83"/>
+      <c r="E3" s="85">
+        <f>DATE(2019, 11, 17)</f>
+        <v>43786</v>
+      </c>
+      <c r="F3" s="85"/>
     </row>
     <row r="4" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="59" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="87" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="88"/>
+        <v>31</v>
+      </c>
+      <c r="C4" s="82" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="83"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="84">
-        <f ca="1">I5</f>
+      <c r="I4" s="86">
+        <f>I5</f>
         <v>43787</v>
       </c>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
-      <c r="L4" s="85"/>
-      <c r="M4" s="85"/>
-      <c r="N4" s="85"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="84">
-        <f ca="1">P5</f>
+      <c r="J4" s="87"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="87"/>
+      <c r="M4" s="87"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="88"/>
+      <c r="P4" s="86">
+        <f>P5</f>
         <v>43794</v>
       </c>
-      <c r="Q4" s="85"/>
-      <c r="R4" s="85"/>
-      <c r="S4" s="85"/>
-      <c r="T4" s="85"/>
-      <c r="U4" s="85"/>
-      <c r="V4" s="86"/>
-      <c r="W4" s="84">
-        <f ca="1">W5</f>
+      <c r="Q4" s="87"/>
+      <c r="R4" s="87"/>
+      <c r="S4" s="87"/>
+      <c r="T4" s="87"/>
+      <c r="U4" s="87"/>
+      <c r="V4" s="88"/>
+      <c r="W4" s="86">
+        <f>W5</f>
         <v>43801</v>
       </c>
-      <c r="X4" s="85"/>
-      <c r="Y4" s="85"/>
-      <c r="Z4" s="85"/>
-      <c r="AA4" s="85"/>
-      <c r="AB4" s="85"/>
-      <c r="AC4" s="86"/>
-      <c r="AD4" s="84">
-        <f ca="1">AD5</f>
+      <c r="X4" s="87"/>
+      <c r="Y4" s="87"/>
+      <c r="Z4" s="87"/>
+      <c r="AA4" s="87"/>
+      <c r="AB4" s="87"/>
+      <c r="AC4" s="88"/>
+      <c r="AD4" s="86">
+        <f>AD5</f>
         <v>43808</v>
       </c>
-      <c r="AE4" s="85"/>
-      <c r="AF4" s="85"/>
-      <c r="AG4" s="85"/>
-      <c r="AH4" s="85"/>
-      <c r="AI4" s="85"/>
-      <c r="AJ4" s="86"/>
+      <c r="AE4" s="87"/>
+      <c r="AF4" s="87"/>
+      <c r="AG4" s="87"/>
+      <c r="AH4" s="87"/>
+      <c r="AI4" s="87"/>
+      <c r="AJ4" s="88"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="59" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
+        <v>32</v>
+      </c>
+      <c r="B5" s="84"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
       <c r="I5" s="11">
-        <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
+        <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43787</v>
       </c>
       <c r="J5" s="10">
-        <f ca="1">I5+1</f>
+        <f>I5+1</f>
         <v>43788</v>
       </c>
       <c r="K5" s="10">
-        <f t="shared" ref="K5:AJ5" ca="1" si="0">J5+1</f>
+        <f t="shared" ref="K5:AJ5" si="0">J5+1</f>
         <v>43789</v>
       </c>
       <c r="L5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43790</v>
       </c>
       <c r="M5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43791</v>
       </c>
       <c r="N5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43792</v>
       </c>
       <c r="O5" s="12">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43793</v>
       </c>
       <c r="P5" s="11">
-        <f ca="1">O5+1</f>
+        <f>O5+1</f>
         <v>43794</v>
       </c>
       <c r="Q5" s="10">
-        <f ca="1">P5+1</f>
+        <f>P5+1</f>
         <v>43795</v>
       </c>
       <c r="R5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43796</v>
       </c>
       <c r="S5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43797</v>
       </c>
       <c r="T5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43798</v>
       </c>
       <c r="U5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43799</v>
       </c>
       <c r="V5" s="12">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43800</v>
       </c>
       <c r="W5" s="11">
-        <f ca="1">V5+1</f>
+        <f>V5+1</f>
         <v>43801</v>
       </c>
       <c r="X5" s="10">
-        <f ca="1">W5+1</f>
+        <f>W5+1</f>
         <v>43802</v>
       </c>
       <c r="Y5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43803</v>
       </c>
       <c r="Z5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43804</v>
       </c>
       <c r="AA5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43805</v>
       </c>
       <c r="AB5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43806</v>
       </c>
       <c r="AC5" s="12">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43807</v>
       </c>
       <c r="AD5" s="11">
-        <f ca="1">AC5+1</f>
+        <f>AC5+1</f>
         <v>43808</v>
       </c>
       <c r="AE5" s="10">
-        <f ca="1">AD5+1</f>
+        <f>AD5+1</f>
         <v>43809</v>
       </c>
       <c r="AF5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43810</v>
       </c>
       <c r="AG5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43811</v>
       </c>
       <c r="AH5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43812</v>
       </c>
       <c r="AI5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43813</v>
       </c>
       <c r="AJ5" s="12">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43814</v>
       </c>
     </row>
     <row r="6" spans="1:36" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="59" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I6" s="13" t="str">
-        <f t="shared" ref="I6" ca="1" si="1">LEFT(TEXT(I5,"ddd"),1)</f>
+        <f t="shared" ref="I6" si="1">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
       </c>
       <c r="J6" s="13" t="str">
-        <f t="shared" ref="J6:AJ6" ca="1" si="2">LEFT(TEXT(J5,"ddd"),1)</f>
+        <f t="shared" ref="J6:AJ6" si="2">LEFT(TEXT(J5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="K6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>W</v>
       </c>
       <c r="L6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>T</v>
       </c>
       <c r="M6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>F</v>
       </c>
       <c r="N6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="O6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="P6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>M</v>
       </c>
       <c r="Q6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>T</v>
       </c>
       <c r="R6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>W</v>
       </c>
       <c r="S6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>T</v>
       </c>
       <c r="T6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>F</v>
       </c>
       <c r="U6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="V6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="W6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>M</v>
       </c>
       <c r="X6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>T</v>
       </c>
       <c r="Y6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>W</v>
       </c>
       <c r="Z6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>T</v>
       </c>
       <c r="AA6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>F</v>
       </c>
       <c r="AB6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="AC6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="AD6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>M</v>
       </c>
       <c r="AE6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>T</v>
       </c>
       <c r="AF6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>W</v>
       </c>
       <c r="AG6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>T</v>
       </c>
       <c r="AH6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>F</v>
       </c>
       <c r="AI6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="AJ6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
     </row>
     <row r="7" spans="1:36" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C7" s="62"/>
       <c r="E7"/>
@@ -1951,13 +1984,13 @@
     </row>
     <row r="8" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="59" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="82" t="s">
-        <v>49</v>
+        <v>52</v>
+      </c>
+      <c r="C8" s="79" t="s">
+        <v>44</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="20"/>
@@ -1998,28 +2031,28 @@
     </row>
     <row r="9" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="59" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="81" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="80" t="s">
-        <v>46</v>
+        <v>35</v>
+      </c>
+      <c r="B9" s="78" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="77" t="s">
+        <v>41</v>
       </c>
       <c r="D9" s="22">
         <v>1</v>
       </c>
       <c r="E9" s="65">
-        <f ca="1">Project_Start</f>
-        <v>43792</v>
+        <f>Project_Start</f>
+        <v>43786</v>
       </c>
       <c r="F9" s="65">
-        <f ca="1">E9+7</f>
-        <v>43799</v>
+        <f>E9+7</f>
+        <v>43793</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I9" s="44"/>
@@ -2053,28 +2086,28 @@
     </row>
     <row r="10" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="81" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="80" t="s">
-        <v>51</v>
+        <v>36</v>
+      </c>
+      <c r="B10" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="77" t="s">
+        <v>46</v>
       </c>
       <c r="D10" s="22">
         <v>0.75</v>
       </c>
       <c r="E10" s="65">
-        <f ca="1">Project_Start</f>
-        <v>43792</v>
+        <f>Project_Start</f>
+        <v>43786</v>
       </c>
       <c r="F10" s="65">
-        <f t="shared" ref="F10:F13" ca="1" si="4">E10+7</f>
-        <v>43799</v>
+        <f t="shared" ref="F10:F13" si="4">E10+7</f>
+        <v>43793</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I10" s="44"/>
@@ -2108,26 +2141,26 @@
     </row>
     <row r="11" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="58"/>
-      <c r="B11" s="81" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="80" t="s">
-        <v>45</v>
+      <c r="B11" s="78" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="77" t="s">
+        <v>40</v>
       </c>
       <c r="D11" s="22">
         <v>0.5</v>
       </c>
       <c r="E11" s="65">
-        <f ca="1">Project_Start</f>
-        <v>43792</v>
+        <f>Project_Start</f>
+        <v>43786</v>
       </c>
       <c r="F11" s="65">
-        <f ca="1">E11+7</f>
-        <v>43799</v>
+        <f>E11+7</f>
+        <v>43793</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="17">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I11" s="44"/>
@@ -2161,26 +2194,26 @@
     </row>
     <row r="12" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="58"/>
-      <c r="B12" s="81" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="80" t="s">
-        <v>47</v>
+      <c r="B12" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="77" t="s">
+        <v>42</v>
       </c>
       <c r="D12" s="22">
         <v>0.9</v>
       </c>
       <c r="E12" s="65">
-        <f ca="1">Project_Start</f>
-        <v>43792</v>
+        <f>Project_Start</f>
+        <v>43786</v>
       </c>
       <c r="F12" s="65">
-        <f t="shared" ca="1" si="4"/>
-        <v>43799</v>
+        <f t="shared" si="4"/>
+        <v>43793</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="17">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I12" s="44"/>
@@ -2214,26 +2247,26 @@
     </row>
     <row r="13" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="58"/>
-      <c r="B13" s="81" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="80" t="s">
-        <v>56</v>
+      <c r="B13" s="78" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="77" t="s">
+        <v>51</v>
       </c>
       <c r="D13" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="65">
-        <f ca="1">Project_Start</f>
-        <v>43792</v>
+        <f>Project_Start</f>
+        <v>43786</v>
       </c>
       <c r="F13" s="65">
-        <f t="shared" ca="1" si="4"/>
-        <v>43799</v>
+        <f t="shared" si="4"/>
+        <v>43793</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="17">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I13" s="44"/>
@@ -2267,10 +2300,10 @@
     </row>
     <row r="14" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="59" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C14" s="70"/>
       <c r="D14" s="24"/>
@@ -2312,26 +2345,26 @@
     </row>
     <row r="15" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="59"/>
-      <c r="B15" s="90" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="91" t="s">
-        <v>47</v>
+      <c r="B15" s="80" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="81" t="s">
+        <v>42</v>
       </c>
       <c r="D15" s="27">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E15" s="66">
-        <f ca="1">$E$13+8</f>
-        <v>43800</v>
+        <f>$E$13+8</f>
+        <v>43794</v>
       </c>
       <c r="F15" s="66">
-        <f ca="1">E15+7</f>
-        <v>43807</v>
+        <f>E15+7</f>
+        <v>43801</v>
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="17">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I15" s="44"/>
@@ -2365,26 +2398,26 @@
     </row>
     <row r="16" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="58"/>
-      <c r="B16" s="90" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="91" t="s">
-        <v>46</v>
+      <c r="B16" s="80" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="81" t="s">
+        <v>41</v>
       </c>
       <c r="D16" s="27">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E16" s="66">
-        <f t="shared" ref="E16:E19" ca="1" si="5">$E$13+8</f>
-        <v>43800</v>
+        <f t="shared" ref="E16:E19" si="5">$E$13+8</f>
+        <v>43794</v>
       </c>
       <c r="F16" s="66">
-        <f t="shared" ref="F16:F19" ca="1" si="6">E16+7</f>
-        <v>43807</v>
+        <f t="shared" ref="F16:F19" si="6">E16+7</f>
+        <v>43801</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="17">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I16" s="44"/>
@@ -2418,26 +2451,26 @@
     </row>
     <row r="17" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="58"/>
-      <c r="B17" s="90" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="91" t="s">
+      <c r="B17" s="80" t="s">
         <v>56</v>
       </c>
+      <c r="C17" s="81" t="s">
+        <v>51</v>
+      </c>
       <c r="D17" s="27">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E17" s="66">
-        <f t="shared" ca="1" si="5"/>
-        <v>43800</v>
+        <f t="shared" si="5"/>
+        <v>43794</v>
       </c>
       <c r="F17" s="66">
-        <f t="shared" ca="1" si="6"/>
-        <v>43807</v>
+        <f t="shared" si="6"/>
+        <v>43801</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I17" s="44"/>
@@ -2471,26 +2504,26 @@
     </row>
     <row r="18" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="58"/>
-      <c r="B18" s="90" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="91" t="s">
-        <v>45</v>
+      <c r="B18" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="81" t="s">
+        <v>51</v>
       </c>
       <c r="D18" s="27">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E18" s="66">
-        <f t="shared" ca="1" si="5"/>
-        <v>43800</v>
+        <f t="shared" si="5"/>
+        <v>43794</v>
       </c>
       <c r="F18" s="66">
-        <f t="shared" ca="1" si="6"/>
-        <v>43807</v>
+        <f t="shared" si="6"/>
+        <v>43801</v>
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="17">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I18" s="44"/>
@@ -2524,26 +2557,26 @@
     </row>
     <row r="19" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="58"/>
-      <c r="B19" s="90" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="91" t="s">
-        <v>56</v>
+      <c r="B19" s="80" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="81" t="s">
+        <v>40</v>
       </c>
       <c r="D19" s="27">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="E19" s="66">
-        <f t="shared" ca="1" si="5"/>
-        <v>43800</v>
+        <f t="shared" si="5"/>
+        <v>43794</v>
       </c>
       <c r="F19" s="66">
-        <f t="shared" ca="1" si="6"/>
-        <v>43807</v>
+        <f t="shared" si="6"/>
+        <v>43801</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="17">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I19" s="44"/>
@@ -2577,10 +2610,10 @@
     </row>
     <row r="20" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="58" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C20" s="71"/>
       <c r="D20" s="29"/>
@@ -2622,22 +2655,26 @@
     </row>
     <row r="21" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="58"/>
-      <c r="B21" s="76" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="72"/>
-      <c r="D21" s="32"/>
+      <c r="B21" s="89" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="90" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="32">
+        <v>0</v>
+      </c>
       <c r="E21" s="67">
-        <f ca="1">$E$9+16</f>
-        <v>43808</v>
+        <f>$E$9+16</f>
+        <v>43802</v>
       </c>
       <c r="F21" s="67">
-        <f ca="1">E21+7</f>
-        <v>43815</v>
+        <f>E21+7</f>
+        <v>43809</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I21" s="44"/>
@@ -2671,22 +2708,26 @@
     </row>
     <row r="22" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="58"/>
-      <c r="B22" s="76" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="72"/>
-      <c r="D22" s="32"/>
+      <c r="B22" s="89" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="90" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="32">
+        <v>0.2</v>
+      </c>
       <c r="E22" s="67">
-        <f t="shared" ref="E22:E25" ca="1" si="7">$E$9+16</f>
-        <v>43808</v>
+        <f t="shared" ref="E22:E25" si="7">$E$9+16</f>
+        <v>43802</v>
       </c>
       <c r="F22" s="67">
-        <f t="shared" ref="F22:F25" ca="1" si="8">E22+7</f>
-        <v>43815</v>
+        <f t="shared" ref="F22:F25" si="8">E22+7</f>
+        <v>43809</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="17">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I22" s="44"/>
@@ -2720,22 +2761,26 @@
     </row>
     <row r="23" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="58"/>
-      <c r="B23" s="76" t="s">
+      <c r="B23" s="89" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="90" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="32">
         <v>0</v>
       </c>
-      <c r="C23" s="72"/>
-      <c r="D23" s="32"/>
       <c r="E23" s="67">
-        <f t="shared" ca="1" si="7"/>
-        <v>43808</v>
+        <f t="shared" si="7"/>
+        <v>43802</v>
       </c>
       <c r="F23" s="67">
-        <f t="shared" ca="1" si="8"/>
-        <v>43815</v>
+        <f t="shared" si="8"/>
+        <v>43809</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="17">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I23" s="44"/>
@@ -2769,22 +2814,24 @@
     </row>
     <row r="24" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="58"/>
-      <c r="B24" s="76" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="72"/>
+      <c r="B24" s="89" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="90" t="s">
+        <v>51</v>
+      </c>
       <c r="D24" s="32"/>
       <c r="E24" s="67">
-        <f t="shared" ca="1" si="7"/>
-        <v>43808</v>
+        <f t="shared" si="7"/>
+        <v>43802</v>
       </c>
       <c r="F24" s="67">
-        <f t="shared" ca="1" si="8"/>
-        <v>43815</v>
+        <f t="shared" si="8"/>
+        <v>43809</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="17">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I24" s="44"/>
@@ -2818,22 +2865,24 @@
     </row>
     <row r="25" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="58"/>
-      <c r="B25" s="76" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" s="72"/>
+      <c r="B25" s="89" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="90" t="s">
+        <v>65</v>
+      </c>
       <c r="D25" s="32"/>
       <c r="E25" s="67">
-        <f t="shared" ca="1" si="7"/>
-        <v>43808</v>
+        <f t="shared" si="7"/>
+        <v>43802</v>
       </c>
       <c r="F25" s="67">
-        <f t="shared" ca="1" si="8"/>
-        <v>43815</v>
+        <f t="shared" si="8"/>
+        <v>43809</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="17">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I25" s="44"/>
@@ -2867,12 +2916,12 @@
     </row>
     <row r="26" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="58" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="73"/>
+        <v>47</v>
+      </c>
+      <c r="C26" s="72"/>
       <c r="D26" s="34"/>
       <c r="E26" s="35"/>
       <c r="F26" s="36"/>
@@ -2912,22 +2961,24 @@
     </row>
     <row r="27" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="58"/>
-      <c r="B27" s="77" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="74"/>
+      <c r="B27" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="92" t="s">
+        <v>61</v>
+      </c>
       <c r="D27" s="37"/>
       <c r="E27" s="68">
-        <f ca="1">$F$25</f>
-        <v>43815</v>
+        <f>$F$25</f>
+        <v>43809</v>
       </c>
       <c r="F27" s="68">
-        <f ca="1">E27+2</f>
-        <v>43817</v>
+        <f>E27+2</f>
+        <v>43811</v>
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="17">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="I27" s="44"/>
@@ -2961,22 +3012,24 @@
     </row>
     <row r="28" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="58"/>
-      <c r="B28" s="77" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="74"/>
+      <c r="B28" s="91" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="92" t="s">
+        <v>46</v>
+      </c>
       <c r="D28" s="37"/>
       <c r="E28" s="68">
-        <f t="shared" ref="E28:E31" ca="1" si="9">$F$25</f>
-        <v>43815</v>
+        <f t="shared" ref="E28:E31" si="9">$F$25</f>
+        <v>43809</v>
       </c>
       <c r="F28" s="68">
-        <f t="shared" ref="F28:F31" ca="1" si="10">E28+2</f>
-        <v>43817</v>
+        <f t="shared" ref="F28:F31" si="10">E28+2</f>
+        <v>43811</v>
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="17">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="I28" s="44"/>
@@ -3010,22 +3063,24 @@
     </row>
     <row r="29" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="58"/>
-      <c r="B29" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="74"/>
+      <c r="B29" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="92" t="s">
+        <v>69</v>
+      </c>
       <c r="D29" s="37"/>
       <c r="E29" s="68">
-        <f t="shared" ca="1" si="9"/>
-        <v>43815</v>
+        <f t="shared" si="9"/>
+        <v>43809</v>
       </c>
       <c r="F29" s="68">
-        <f t="shared" ca="1" si="10"/>
-        <v>43817</v>
+        <f t="shared" si="10"/>
+        <v>43811</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="17">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="I29" s="44"/>
@@ -3059,22 +3114,20 @@
     </row>
     <row r="30" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="58"/>
-      <c r="B30" s="77" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="74"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="73"/>
       <c r="D30" s="37"/>
       <c r="E30" s="68">
-        <f t="shared" ca="1" si="9"/>
-        <v>43815</v>
+        <f t="shared" si="9"/>
+        <v>43809</v>
       </c>
       <c r="F30" s="68">
-        <f t="shared" ca="1" si="10"/>
-        <v>43817</v>
+        <f t="shared" si="10"/>
+        <v>43811</v>
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="17">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="I30" s="44"/>
@@ -3108,22 +3161,20 @@
     </row>
     <row r="31" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="58"/>
-      <c r="B31" s="77" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" s="74"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="73"/>
       <c r="D31" s="37"/>
       <c r="E31" s="68">
-        <f t="shared" ca="1" si="9"/>
-        <v>43815</v>
+        <f t="shared" si="9"/>
+        <v>43809</v>
       </c>
       <c r="F31" s="68">
-        <f t="shared" ca="1" si="10"/>
-        <v>43817</v>
+        <f t="shared" si="10"/>
+        <v>43811</v>
       </c>
       <c r="G31" s="17"/>
       <c r="H31" s="17">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="I31" s="44"/>
@@ -3157,10 +3208,10 @@
     </row>
     <row r="32" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="58" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="78"/>
-      <c r="C32" s="75"/>
+        <v>27</v>
+      </c>
+      <c r="B32" s="76"/>
+      <c r="C32" s="74"/>
       <c r="D32" s="16"/>
       <c r="E32" s="69"/>
       <c r="F32" s="69"/>
@@ -3200,10 +3251,10 @@
     </row>
     <row r="33" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="59" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B33" s="38" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C33" s="39"/>
       <c r="D33" s="40"/>
@@ -3255,14 +3306,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="P4:V4"/>
+    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="AD4:AJ4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="14">
@@ -3354,79 +3405,79 @@
     <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:2" s="50" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="49" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B2" s="49"/>
     </row>
     <row r="3" spans="1:2" s="54" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B3" s="55"/>
     </row>
     <row r="4" spans="1:2" s="51" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A4" s="52" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="74" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="53" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="52" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="48" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="57" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="51" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A8" s="52" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="53" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="48" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="56" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="51" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A11" s="52" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="53" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="48" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="56" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="51" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A14" s="52" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="53" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="53" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added software process model, updated schedule
</commit_message>
<xml_diff>
--- a/documentation/2-planning/Project Schedule.xlsx
+++ b/documentation/2-planning/Project Schedule.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F25D5D5-4616-9541-A92B-45DAD659E378}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FF9ADD-190B-364C-9716-65F38402F6A5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="460" windowWidth="27720" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -240,9 +240,6 @@
     <t>Sprint 2 - Step 3&amp;4a</t>
   </si>
   <si>
-    <t>Step 4</t>
-  </si>
-  <si>
     <t>Begin Database Front-end Functionality</t>
   </si>
   <si>
@@ -264,9 +261,6 @@
     <t>Daniel Watson</t>
   </si>
   <si>
-    <t>Program Statistics Dashboard</t>
-  </si>
-  <si>
     <t>Class Diagram</t>
   </si>
   <si>
@@ -276,9 +270,6 @@
     <t>Jaisal Friedman, Daniel Watson</t>
   </si>
   <si>
-    <t>Bug Report</t>
-  </si>
-  <si>
     <t xml:space="preserve">Finalize Documentation </t>
   </si>
   <si>
@@ -295,6 +286,18 @@
   </si>
   <si>
     <t>Mai Oudah</t>
+  </si>
+  <si>
+    <t>Sprint 4 - Step 4</t>
+  </si>
+  <si>
+    <t>Test Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Launch to Heroku </t>
+  </si>
+  <si>
+    <t>Request to Connect with Mentor Dashboard</t>
   </si>
 </sst>
 </file>
@@ -938,6 +941,30 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="11" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -947,30 +974,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="7" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1571,8 +1574,8 @@
   <dimension ref="A1:AJ36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <pane ySplit="6" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1603,7 +1606,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="14"/>
       <c r="K1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1619,81 +1622,81 @@
       <c r="A3" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="93" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="82" t="s">
+      <c r="B3" s="86" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="83"/>
-      <c r="E3" s="85">
+      <c r="D3" s="91"/>
+      <c r="E3" s="93">
         <f>DATE(2019, 11, 17)</f>
         <v>43786</v>
       </c>
-      <c r="F3" s="85"/>
+      <c r="F3" s="93"/>
     </row>
     <row r="4" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="82" t="s">
+      <c r="C4" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="83"/>
+      <c r="D4" s="91"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="86">
+      <c r="I4" s="87">
         <f>I5</f>
         <v>43787</v>
       </c>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="87"/>
-      <c r="M4" s="87"/>
-      <c r="N4" s="87"/>
-      <c r="O4" s="88"/>
-      <c r="P4" s="86">
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="88"/>
+      <c r="O4" s="89"/>
+      <c r="P4" s="87">
         <f>P5</f>
         <v>43794</v>
       </c>
-      <c r="Q4" s="87"/>
-      <c r="R4" s="87"/>
-      <c r="S4" s="87"/>
-      <c r="T4" s="87"/>
-      <c r="U4" s="87"/>
-      <c r="V4" s="88"/>
-      <c r="W4" s="86">
+      <c r="Q4" s="88"/>
+      <c r="R4" s="88"/>
+      <c r="S4" s="88"/>
+      <c r="T4" s="88"/>
+      <c r="U4" s="88"/>
+      <c r="V4" s="89"/>
+      <c r="W4" s="87">
         <f>W5</f>
         <v>43801</v>
       </c>
-      <c r="X4" s="87"/>
-      <c r="Y4" s="87"/>
-      <c r="Z4" s="87"/>
-      <c r="AA4" s="87"/>
-      <c r="AB4" s="87"/>
-      <c r="AC4" s="88"/>
-      <c r="AD4" s="86">
+      <c r="X4" s="88"/>
+      <c r="Y4" s="88"/>
+      <c r="Z4" s="88"/>
+      <c r="AA4" s="88"/>
+      <c r="AB4" s="88"/>
+      <c r="AC4" s="89"/>
+      <c r="AD4" s="87">
         <f>AD5</f>
         <v>43808</v>
       </c>
-      <c r="AE4" s="87"/>
-      <c r="AF4" s="87"/>
-      <c r="AG4" s="87"/>
-      <c r="AH4" s="87"/>
-      <c r="AI4" s="87"/>
-      <c r="AJ4" s="88"/>
+      <c r="AE4" s="88"/>
+      <c r="AF4" s="88"/>
+      <c r="AG4" s="88"/>
+      <c r="AH4" s="88"/>
+      <c r="AI4" s="88"/>
+      <c r="AJ4" s="89"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43787</v>
@@ -2095,7 +2098,7 @@
         <v>46</v>
       </c>
       <c r="D10" s="22">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E10" s="65">
         <f>Project_Start</f>
@@ -2201,7 +2204,7 @@
         <v>42</v>
       </c>
       <c r="D12" s="22">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E12" s="65">
         <f>Project_Start</f>
@@ -2346,7 +2349,7 @@
     <row r="15" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="59"/>
       <c r="B15" s="80" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="81" t="s">
         <v>42</v>
@@ -2399,13 +2402,13 @@
     <row r="16" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="58"/>
       <c r="B16" s="80" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="81" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="27">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E16" s="66">
         <f t="shared" ref="E16:E19" si="5">$E$13+8</f>
@@ -2452,7 +2455,7 @@
     <row r="17" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="58"/>
       <c r="B17" s="80" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="81" t="s">
         <v>51</v>
@@ -2505,7 +2508,7 @@
     <row r="18" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="58"/>
       <c r="B18" s="80" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="81" t="s">
         <v>51</v>
@@ -2558,7 +2561,7 @@
     <row r="19" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="58"/>
       <c r="B19" s="80" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C19" s="81" t="s">
         <v>40</v>
@@ -2613,7 +2616,7 @@
         <v>25</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="C20" s="71"/>
       <c r="D20" s="29"/>
@@ -2655,14 +2658,14 @@
     </row>
     <row r="21" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="58"/>
-      <c r="B21" s="89" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="90" t="s">
+      <c r="B21" s="82" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="83" t="s">
         <v>40</v>
       </c>
       <c r="D21" s="32">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E21" s="67">
         <f>$E$9+16</f>
@@ -2708,14 +2711,14 @@
     </row>
     <row r="22" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="58"/>
-      <c r="B22" s="89" t="s">
+      <c r="B22" s="82" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="90" t="s">
-        <v>61</v>
-      </c>
       <c r="D22" s="32">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="67">
         <f t="shared" ref="E22:E25" si="7">$E$9+16</f>
@@ -2761,14 +2764,14 @@
     </row>
     <row r="23" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="58"/>
-      <c r="B23" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="90" t="s">
-        <v>40</v>
+      <c r="B23" s="82" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="83" t="s">
+        <v>42</v>
       </c>
       <c r="D23" s="32">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E23" s="67">
         <f t="shared" si="7"/>
@@ -2814,13 +2817,15 @@
     </row>
     <row r="24" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="58"/>
-      <c r="B24" s="89" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="90" t="s">
+      <c r="B24" s="82" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="32"/>
+      <c r="D24" s="32">
+        <v>1</v>
+      </c>
       <c r="E24" s="67">
         <f t="shared" si="7"/>
         <v>43802</v>
@@ -2865,13 +2870,15 @@
     </row>
     <row r="25" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="58"/>
-      <c r="B25" s="89" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="90" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="32"/>
+      <c r="B25" s="82" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="83" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="32">
+        <v>0.8</v>
+      </c>
       <c r="E25" s="67">
         <f t="shared" si="7"/>
         <v>43802</v>
@@ -2961,11 +2968,11 @@
     </row>
     <row r="27" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="58"/>
-      <c r="B27" s="91" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="92" t="s">
-        <v>61</v>
+      <c r="B27" s="84" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="85" t="s">
+        <v>60</v>
       </c>
       <c r="D27" s="37"/>
       <c r="E27" s="68">
@@ -3012,13 +3019,15 @@
     </row>
     <row r="28" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="58"/>
-      <c r="B28" s="91" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="92" t="s">
+      <c r="B28" s="84" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="37"/>
+      <c r="D28" s="37">
+        <v>0.2</v>
+      </c>
       <c r="E28" s="68">
         <f t="shared" ref="E28:E31" si="9">$F$25</f>
         <v>43809</v>
@@ -3063,11 +3072,11 @@
     </row>
     <row r="29" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="58"/>
-      <c r="B29" s="91" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" s="92" t="s">
-        <v>69</v>
+      <c r="B29" s="84" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="85" t="s">
+        <v>66</v>
       </c>
       <c r="D29" s="37"/>
       <c r="E29" s="68">
@@ -3114,8 +3123,12 @@
     </row>
     <row r="30" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="58"/>
-      <c r="B30" s="75"/>
-      <c r="C30" s="73"/>
+      <c r="B30" s="84" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="85" t="s">
+        <v>40</v>
+      </c>
       <c r="D30" s="37"/>
       <c r="E30" s="68">
         <f t="shared" si="9"/>
@@ -3306,14 +3319,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="I4:O4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="14">

</xml_diff>

<commit_message>
updated schedule, added risk table, added test case outcomes
</commit_message>
<xml_diff>
--- a/documentation/2-planning/Project Schedule.xlsx
+++ b/documentation/2-planning/Project Schedule.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FF9ADD-190B-364C-9716-65F38402F6A5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2E6ED1-0359-724D-91C9-5CDD7D2EFB28}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="460" windowWidth="27720" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1100" yWindow="460" windowWidth="27700" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -956,6 +956,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -970,10 +974,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1574,8 +1574,8 @@
   <dimension ref="A1:AJ36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
+      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1625,78 +1625,78 @@
       <c r="B3" s="86" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="91"/>
-      <c r="E3" s="93">
+      <c r="D3" s="93"/>
+      <c r="E3" s="88">
         <f>DATE(2019, 11, 17)</f>
         <v>43786</v>
       </c>
-      <c r="F3" s="93"/>
+      <c r="F3" s="88"/>
     </row>
     <row r="4" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="90" t="s">
+      <c r="C4" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="91"/>
+      <c r="D4" s="93"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="87">
+      <c r="I4" s="89">
         <f>I5</f>
         <v>43787</v>
       </c>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="89"/>
-      <c r="P4" s="87">
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="89">
         <f>P5</f>
         <v>43794</v>
       </c>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="88"/>
-      <c r="V4" s="89"/>
-      <c r="W4" s="87">
+      <c r="Q4" s="90"/>
+      <c r="R4" s="90"/>
+      <c r="S4" s="90"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="90"/>
+      <c r="V4" s="91"/>
+      <c r="W4" s="89">
         <f>W5</f>
         <v>43801</v>
       </c>
-      <c r="X4" s="88"/>
-      <c r="Y4" s="88"/>
-      <c r="Z4" s="88"/>
-      <c r="AA4" s="88"/>
-      <c r="AB4" s="88"/>
-      <c r="AC4" s="89"/>
-      <c r="AD4" s="87">
+      <c r="X4" s="90"/>
+      <c r="Y4" s="90"/>
+      <c r="Z4" s="90"/>
+      <c r="AA4" s="90"/>
+      <c r="AB4" s="90"/>
+      <c r="AC4" s="91"/>
+      <c r="AD4" s="89">
         <f>AD5</f>
         <v>43808</v>
       </c>
-      <c r="AE4" s="88"/>
-      <c r="AF4" s="88"/>
-      <c r="AG4" s="88"/>
-      <c r="AH4" s="88"/>
-      <c r="AI4" s="88"/>
-      <c r="AJ4" s="89"/>
+      <c r="AE4" s="90"/>
+      <c r="AF4" s="90"/>
+      <c r="AG4" s="90"/>
+      <c r="AH4" s="90"/>
+      <c r="AI4" s="90"/>
+      <c r="AJ4" s="91"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="92"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43787</v>
@@ -2151,7 +2151,7 @@
         <v>40</v>
       </c>
       <c r="D11" s="22">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E11" s="65">
         <f>Project_Start</f>
@@ -2461,7 +2461,7 @@
         <v>51</v>
       </c>
       <c r="D17" s="27">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E17" s="66">
         <f t="shared" si="5"/>
@@ -2514,7 +2514,7 @@
         <v>51</v>
       </c>
       <c r="D18" s="27">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E18" s="66">
         <f t="shared" si="5"/>
@@ -2665,7 +2665,7 @@
         <v>40</v>
       </c>
       <c r="D21" s="32">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E21" s="67">
         <f>$E$9+16</f>
@@ -2771,7 +2771,7 @@
         <v>42</v>
       </c>
       <c r="D23" s="32">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E23" s="67">
         <f t="shared" si="7"/>
@@ -2877,7 +2877,7 @@
         <v>63</v>
       </c>
       <c r="D25" s="32">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E25" s="67">
         <f t="shared" si="7"/>
@@ -2974,7 +2974,9 @@
       <c r="C27" s="85" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="37"/>
+      <c r="D27" s="37">
+        <v>1</v>
+      </c>
       <c r="E27" s="68">
         <f>$F$25</f>
         <v>43809</v>
@@ -3026,7 +3028,7 @@
         <v>46</v>
       </c>
       <c r="D28" s="37">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E28" s="68">
         <f t="shared" ref="E28:E31" si="9">$F$25</f>
@@ -3078,7 +3080,9 @@
       <c r="C29" s="85" t="s">
         <v>66</v>
       </c>
-      <c r="D29" s="37"/>
+      <c r="D29" s="37">
+        <v>1</v>
+      </c>
       <c r="E29" s="68">
         <f t="shared" si="9"/>
         <v>43809</v>
@@ -3129,7 +3133,9 @@
       <c r="C30" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="37"/>
+      <c r="D30" s="37">
+        <v>0.4</v>
+      </c>
       <c r="E30" s="68">
         <f t="shared" si="9"/>
         <v>43809</v>
@@ -3319,14 +3325,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="14">

</xml_diff>